<commit_message>
Documentation moved to folder, stats library sans calc
</commit_message>
<xml_diff>
--- a/src/StockBot/DataFiles/Graphs/RSI5smooth5appleDaily.xlsx
+++ b/src/StockBot/DataFiles/Graphs/RSI5smooth5appleDaily.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dustin\IdeaProjects\Project_2\src\StockBot\DataFiles\Graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{98F11A7F-EDC4-4357-AF76-31079E72E3D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCF5E75-C9DE-4CF4-A465-C68C6F9AC369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="2700" windowWidth="28800" windowHeight="15435"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RSI5smooth5appleDaily" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -626,7 +626,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Apple Daily with Moving Average</a:t>
+              <a:t>Apple Daily with Moving Average 5</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -6437,9 +6437,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1048565"/>
-                <c:pt idx="0">
-                  <c:v>63.098161178528699</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>73.445870937216895</c:v>
                 </c:pt>
@@ -8876,11 +8873,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="X30" sqref="X30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AE24" sqref="AE24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9202,9 +9199,6 @@
       <c r="H12">
         <v>172.385882363636</v>
       </c>
-      <c r="I12">
-        <v>63.098161178528699</v>
-      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">

</xml_diff>